<commit_message>
Revert "Guion 1 final"
This reverts commit a8d763c4b791c3c8e805797f14a5db946c46980f.
</commit_message>
<xml_diff>
--- a/seguimiento/Grado05.xlsx
+++ b/seguimiento/Grado05.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="13875" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="3120" yWindow="13880" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Seguimiento" sheetId="1" r:id="rId1"/>
@@ -821,7 +821,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -832,43 +832,43 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
-    <col min="2" max="5" width="11.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="6.1640625" style="1" customWidth="1"/>
+    <col min="2" max="5" width="11.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
       <c r="B1" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="34"/>
     </row>
-    <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="16" thickBot="1">
       <c r="B2" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="35"/>
       <c r="D2" s="36"/>
     </row>
-    <row r="3" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="16" thickBot="1">
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A4" s="37" t="s">
         <v>4</v>
       </c>
@@ -892,7 +892,7 @@
       </c>
       <c r="L4" s="32"/>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="29" thickBot="1">
       <c r="A5" s="37"/>
       <c r="B5" s="22" t="s">
         <v>2</v>
@@ -928,13 +928,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="16" thickBot="1">
       <c r="A6" s="29">
         <v>1</v>
       </c>
-      <c r="B6" s="4">
-        <v>42079</v>
-      </c>
+      <c r="B6" s="4"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -948,7 +946,7 @@
       <c r="K6" s="14"/>
       <c r="L6" s="15"/>
     </row>
-    <row r="7" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="16" thickBot="1">
       <c r="A7" s="29">
         <v>2</v>
       </c>
@@ -964,7 +962,7 @@
       <c r="K7" s="14"/>
       <c r="L7" s="15"/>
     </row>
-    <row r="8" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" s="29">
         <v>3</v>
       </c>
@@ -980,7 +978,7 @@
       <c r="K8" s="14"/>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="16" thickBot="1">
       <c r="A9" s="29">
         <v>4</v>
       </c>
@@ -996,7 +994,7 @@
       <c r="K9" s="14"/>
       <c r="L9" s="15"/>
     </row>
-    <row r="10" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" s="29">
         <v>5</v>
       </c>
@@ -1012,7 +1010,7 @@
       <c r="K10" s="14"/>
       <c r="L10" s="15"/>
     </row>
-    <row r="11" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="29">
         <v>6</v>
       </c>
@@ -1028,7 +1026,7 @@
       <c r="K11" s="14"/>
       <c r="L11" s="15"/>
     </row>
-    <row r="12" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="16" thickBot="1">
       <c r="A12" s="29">
         <v>7</v>
       </c>
@@ -1044,7 +1042,7 @@
       <c r="K12" s="14"/>
       <c r="L12" s="15"/>
     </row>
-    <row r="13" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="16" thickBot="1">
       <c r="A13" s="29">
         <v>8</v>
       </c>
@@ -1060,7 +1058,7 @@
       <c r="K13" s="14"/>
       <c r="L13" s="15"/>
     </row>
-    <row r="14" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="16" thickBot="1">
       <c r="A14" s="29">
         <v>9</v>
       </c>
@@ -1076,7 +1074,7 @@
       <c r="K14" s="14"/>
       <c r="L14" s="15"/>
     </row>
-    <row r="15" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="16" thickBot="1">
       <c r="A15" s="29">
         <v>10</v>
       </c>
@@ -1092,7 +1090,7 @@
       <c r="K15" s="14"/>
       <c r="L15" s="15"/>
     </row>
-    <row r="16" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="16" thickBot="1">
       <c r="A16" s="29">
         <v>11</v>
       </c>
@@ -1108,7 +1106,7 @@
       <c r="K16" s="14"/>
       <c r="L16" s="15"/>
     </row>
-    <row r="17" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="16" thickBot="1">
       <c r="A17" s="29">
         <v>12</v>
       </c>
@@ -1124,7 +1122,7 @@
       <c r="K17" s="14"/>
       <c r="L17" s="15"/>
     </row>
-    <row r="18" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="16" thickBot="1">
       <c r="A18" s="29">
         <v>13</v>
       </c>
@@ -1140,7 +1138,7 @@
       <c r="K18" s="14"/>
       <c r="L18" s="15"/>
     </row>
-    <row r="19" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19" s="29">
         <v>14</v>
       </c>
@@ -1156,7 +1154,7 @@
       <c r="K19" s="14"/>
       <c r="L19" s="15"/>
     </row>
-    <row r="20" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="16" thickBot="1">
       <c r="A20" s="29">
         <v>15</v>
       </c>
@@ -1172,7 +1170,7 @@
       <c r="K20" s="14"/>
       <c r="L20" s="15"/>
     </row>
-    <row r="21" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="30">
         <v>16</v>
       </c>

</xml_diff>